<commit_message>
2021 stats course added
</commit_message>
<xml_diff>
--- a/Teaching_Overview.xlsx
+++ b/Teaching_Overview.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\R\brry.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D42896E8-2D67-4C5B-AAE7-882C01E383C2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42921574-7190-45A5-98D3-189CEA26F451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16320" yWindow="-7905" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -162,7 +162,8 @@
     <t>[2017](https://swc-bb.github.io/2017-05-17-GFZ), [18](https://swc-bb.github.io/2018-04-25-Potsdam-Berlin), [19](https://swc-bb.github.io/2019-11-26-Potsdam-Berlin-R)</t>
   </si>
   <si>
-    <t>[2020](https://open.hpi.de/courses/StatisticsCHealthSoSe2020)</t>
+    <t>[2020](https://open.hpi.de/courses/StatisticsCHealthSoSe2020) + 
+[2021](https://open.hpi.de/courses/hpi-dh-StatisticsCHealth2021)</t>
   </si>
 </sst>
 </file>
@@ -222,7 +223,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -238,7 +239,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -540,7 +541,7 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="76.42578125" style="2" customWidth="1"/>

</xml_diff>